<commit_message>
Removed FAQ from repo
</commit_message>
<xml_diff>
--- a/Cycle Project.xlsx
+++ b/Cycle Project.xlsx
@@ -1060,7 +1060,7 @@
   <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="1">
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A25" workbookViewId="1">
       <selection activeCell="C80" sqref="A2:C80"/>
     </sheetView>
   </sheetViews>
@@ -1774,6 +1774,10 @@
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;D&amp;CThe Cycle Project_x000D_Budget Projection&amp;RJake Zerrer</oddHeader>
+    <oddFooter>&amp;R&amp;P of &amp;N</oddFooter>
+  </headerFooter>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>